<commit_message>
Fixed PD & Enforcements sheets
</commit_message>
<xml_diff>
--- a/Templates/Dropbox_v2.xlsx
+++ b/Templates/Dropbox_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="8" r:id="rId1"/>
@@ -412,27 +412,18 @@
     <t>Account Information</t>
   </si>
   <si>
-    <t>name, email, phone number, payment info, and physical address</t>
-  </si>
-  <si>
     <t>Device Information</t>
   </si>
   <si>
     <t>Location Information</t>
   </si>
   <si>
-    <t>IP addresses, the type of browser and device you use, the web page you visited before coming to our sites, and identifiers associated with your devices.</t>
-  </si>
-  <si>
     <t>location information</t>
   </si>
   <si>
     <t>Files</t>
   </si>
   <si>
-    <t>photos, structured data and emails</t>
-  </si>
-  <si>
     <t>File-related Information</t>
   </si>
   <si>
@@ -641,6 +632,15 @@
   </si>
   <si>
     <t>Enforcements</t>
+  </si>
+  <si>
+    <t>photos, structured data, emails</t>
+  </si>
+  <si>
+    <t>IP addresses, the type of browser and device you use, the web page you visited before coming to our sites, identifiers associated with your devices.</t>
+  </si>
+  <si>
+    <t>name, email, phone number, payment info, physical address</t>
   </si>
 </sst>
 </file>
@@ -887,7 +887,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -952,18 +952,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1344,72 +1332,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="49" t="s">
+      <c r="B5" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="50" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>181</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="49" t="s">
+      <c r="B6" s="45">
+        <v>42412</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="B4" s="50" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="49" t="s">
-        <v>177</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>180</v>
-      </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="B6" s="51">
-        <v>42412</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="49" t="s">
+      <c r="B7" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1420,7 +1408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1431,51 +1419,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21">
-      <c r="A1" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="A1" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:4" ht="21">
-      <c r="A2" s="52" t="s">
-        <v>184</v>
+      <c r="A2" s="46" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="47" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="53" t="s">
-        <v>201</v>
+      <c r="A5" s="47" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="47" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="47" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="53" t="s">
-        <v>202</v>
+      <c r="A8" s="47" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="53" t="s">
-        <v>185</v>
+      <c r="A9" s="47" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="53" t="s">
-        <v>186</v>
+      <c r="A10" s="47" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1494,17 +1482,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J95"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="170.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" style="4" customWidth="1"/>
@@ -1530,20 +1518,20 @@
       <c r="E1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="48" t="s">
         <v>15</v>
       </c>
       <c r="G1" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" s="28" t="s">
         <v>187</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1627,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
@@ -1651,13 +1639,13 @@
         <v>0</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G6" s="10">
         <v>7</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I6" s="21"/>
       <c r="J6" s="22"/>
@@ -1677,13 +1665,13 @@
         <v>0</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G7" s="10">
         <v>2</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="22"/>
@@ -1727,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G9" s="10">
         <v>2</v>
@@ -1775,13 +1763,13 @@
         <v>0</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G11" s="10">
         <v>5</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I11" s="21"/>
       <c r="J11" s="22"/>
@@ -1801,13 +1789,13 @@
         <v>0</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G12" s="10">
         <v>5</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I12" s="21"/>
       <c r="J12" s="22"/>
@@ -1827,13 +1815,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G13" s="10">
         <v>5</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="22"/>
@@ -1853,13 +1841,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G14" s="10">
         <v>5</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="22"/>
@@ -1879,13 +1867,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G15" s="10">
         <v>7</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="22"/>
@@ -1905,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G16" s="10">
         <v>6</v>
@@ -1929,15 +1917,15 @@
         <v>1</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1961,7 +1949,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="21"/>
       <c r="J18" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1979,15 +1967,15 @@
         <v>1</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I19" s="21"/>
       <c r="J19" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2005,13 +1993,13 @@
         <v>1</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="21"/>
       <c r="J20" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1">
@@ -2029,15 +2017,15 @@
         <v>1</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I21" s="21"/>
       <c r="J21" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1">
@@ -2055,15 +2043,15 @@
         <v>1</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1">
@@ -2081,13 +2069,13 @@
         <v>1</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="21"/>
       <c r="J23" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1">
@@ -2105,11 +2093,11 @@
         <v>3</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I24" s="21"/>
       <c r="J24" s="22"/>
@@ -2129,11 +2117,11 @@
         <v>3</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I25" s="21"/>
       <c r="J25" s="22"/>
@@ -2215,7 +2203,7 @@
         <v>13</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -2508,428 +2496,12 @@
       <c r="I43" s="24"/>
       <c r="J43" s="25"/>
     </row>
-    <row r="44" spans="1:10" ht="15" customHeight="1">
-      <c r="A44" s="30"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="33"/>
-    </row>
-    <row r="45" spans="1:10" ht="15" customHeight="1">
-      <c r="A45" s="30"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="33"/>
-    </row>
-    <row r="46" spans="1:10" ht="15" customHeight="1">
-      <c r="A46" s="30"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="33"/>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="30"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="33"/>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="30"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="33"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="30"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="33"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="30"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="33"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="30"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="33"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="30"/>
-      <c r="B52" s="31"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="33"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="30"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="33"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="30"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="33"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="30"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="33"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="30"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="33"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="30"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="33"/>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="30"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="33"/>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="30"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="33"/>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="30"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="33"/>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="30"/>
-      <c r="B61" s="31"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="33"/>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="30"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="33"/>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="30"/>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="33"/>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="30"/>
-      <c r="B64" s="32"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="33"/>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="30"/>
-      <c r="B65" s="32"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="33"/>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="30"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="33"/>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="30"/>
-      <c r="B67" s="31"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="33"/>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="30"/>
-      <c r="B68" s="31"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="33"/>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="30"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="33"/>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="30"/>
-      <c r="B70" s="32"/>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="33"/>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="30"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="33"/>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="30"/>
-      <c r="B72" s="31"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="33"/>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="30"/>
-      <c r="B73" s="31"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="33"/>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="30"/>
-      <c r="B74" s="31"/>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="32"/>
-      <c r="F74" s="33"/>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="30"/>
-      <c r="B75" s="31"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="33"/>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="30"/>
-      <c r="B76" s="31"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="33"/>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="30"/>
-      <c r="B77" s="31"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="33"/>
-    </row>
-    <row r="78" spans="1:6" ht="33" customHeight="1">
-      <c r="A78" s="30"/>
-      <c r="B78" s="31"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="33"/>
-    </row>
-    <row r="79" spans="1:6" ht="33" customHeight="1">
-      <c r="A79" s="30"/>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32"/>
-      <c r="D79" s="32"/>
-      <c r="E79" s="32"/>
-      <c r="F79" s="33"/>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="30"/>
-      <c r="B80" s="32"/>
-      <c r="C80" s="32"/>
-      <c r="D80" s="32"/>
-      <c r="E80" s="32"/>
-      <c r="F80" s="33"/>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" s="30"/>
-      <c r="B81" s="32"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="32"/>
-      <c r="F81" s="33"/>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="30"/>
-      <c r="B82" s="32"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32"/>
-      <c r="E82" s="32"/>
-      <c r="F82" s="33"/>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="30"/>
-      <c r="B83" s="31"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="32"/>
-      <c r="E83" s="32"/>
-      <c r="F83" s="33"/>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="30"/>
-      <c r="B84" s="32"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="32"/>
-      <c r="E84" s="32"/>
-      <c r="F84" s="33"/>
-    </row>
-    <row r="85" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A85" s="30"/>
-      <c r="B85" s="32"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="32"/>
-      <c r="F85" s="33"/>
-    </row>
-    <row r="86" spans="1:6" ht="48" customHeight="1">
-      <c r="A86" s="30"/>
-      <c r="B86" s="32"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="33"/>
-    </row>
-    <row r="87" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A87" s="30"/>
-      <c r="B87" s="32"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="32"/>
-      <c r="F87" s="33"/>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="30"/>
-      <c r="B88" s="32"/>
-      <c r="C88" s="32"/>
-      <c r="D88" s="32"/>
-      <c r="E88" s="32"/>
-      <c r="F88" s="33"/>
-    </row>
-    <row r="89" spans="1:6" ht="33" customHeight="1">
-      <c r="A89" s="30"/>
-      <c r="B89" s="31"/>
-      <c r="C89" s="32"/>
-      <c r="D89" s="32"/>
-      <c r="E89" s="32"/>
-      <c r="F89" s="33"/>
-    </row>
-    <row r="90" spans="1:6" ht="33" customHeight="1">
-      <c r="A90" s="30"/>
-      <c r="B90" s="32"/>
-      <c r="C90" s="32"/>
-      <c r="D90" s="32"/>
-      <c r="E90" s="32"/>
-      <c r="F90" s="33"/>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" s="34"/>
-      <c r="B91" s="34"/>
-      <c r="C91" s="34"/>
-      <c r="D91" s="34"/>
-      <c r="E91" s="34"/>
-      <c r="F91" s="33"/>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92" s="34"/>
-      <c r="B92" s="34"/>
-      <c r="C92" s="34"/>
-      <c r="D92" s="34"/>
-      <c r="E92" s="34"/>
-      <c r="F92" s="33"/>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" s="34"/>
-      <c r="B93" s="35"/>
-      <c r="C93" s="34"/>
-      <c r="D93" s="34"/>
-      <c r="E93" s="34"/>
-      <c r="F93" s="33"/>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="34"/>
-      <c r="B94" s="34"/>
-      <c r="C94" s="34"/>
-      <c r="D94" s="34"/>
-      <c r="E94" s="34"/>
-      <c r="F94" s="33"/>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="34"/>
-      <c r="B95" s="34"/>
-      <c r="C95" s="34"/>
-      <c r="D95" s="34"/>
-      <c r="E95" s="34"/>
-      <c r="F95" s="33"/>
-    </row>
   </sheetData>
   <sortState ref="A2:F93">
     <sortCondition ref="E2:E93" customList="Collection,Disclosure,Retention,Usage,Informative"/>
   </sortState>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E90">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E43">
       <formula1>statements_type</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D43">
@@ -2972,7 +2544,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2980,7 +2552,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>21</v>
@@ -2995,7 +2567,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>20</v>
@@ -3010,7 +2582,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>19</v>
@@ -3025,7 +2597,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>21</v>
@@ -3040,7 +2612,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>20</v>
@@ -3054,8 +2626,8 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>150</v>
+      <c r="B7" s="30" t="s">
+        <v>147</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>19</v>
@@ -3070,7 +2642,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>21</v>
@@ -3082,7 +2654,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3101,9 +2673,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD131"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3128,129 +2702,129 @@
         <v>15</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="40">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="55"/>
+      <c r="B2" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="38">
+      <c r="A3" s="32">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E3" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="38">
+      <c r="A4" s="32">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E4" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="38">
+      <c r="A5" s="32">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E5" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="40">
+      <c r="A6" s="34">
         <v>5</v>
       </c>
-      <c r="B6" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="55"/>
+      <c r="B6" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="49"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="38">
+      <c r="A7" s="32">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E7" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="38">
+      <c r="A8" s="32">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E8" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="38">
+      <c r="A9" s="32">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="22">
@@ -3258,57 +2832,51 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="40">
+      <c r="A10" s="34">
         <v>9</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="49"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="33">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" s="55"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="39">
-        <v>10</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>159</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E11" s="22">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="39">
+      <c r="A12" s="33">
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E12" s="25">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="34"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3321,14 +2889,14 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="114" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3337,10 +2905,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>14</v>
@@ -3351,13 +2919,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" s="13" t="s">
-        <v>126</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
@@ -3365,13 +2933,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>129</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
@@ -3379,13 +2947,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>128</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
@@ -3393,13 +2961,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>131</v>
+        <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>11</v>
+        <v>129</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
@@ -3407,13 +2975,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
@@ -3421,13 +2989,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>137</v>
+        <v>11</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>11</v>
+        <v>134</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
@@ -3435,13 +3003,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>138</v>
+        <v>11</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
@@ -3449,18 +3017,18 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B9">
       <formula1>privatedata_type</formula1>
     </dataValidation>
   </dataValidations>
@@ -3470,9 +3038,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3503,7 +3071,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>87</v>
@@ -3517,7 +3085,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>89</v>
@@ -3531,7 +3099,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>105</v>
@@ -3545,24 +3113,18 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="C5" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="31" t="s">
         <v>106</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="34"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D6">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D5">
       <formula1>enforcement_type</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>